<commit_message>
Object before Nov 9, Fri.
</commit_message>
<xml_diff>
--- a/331GRADES.xlsx
+++ b/331GRADES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Furkan\Desktop\331\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E373AC4F-1F45-40CD-90DF-1E9EFB965E88}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAAF99F4-5C7A-4775-A612-542B000B4132}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,7 +640,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -652,15 +652,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1016,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,68 +1033,68 @@
     <col min="8" max="8" width="11.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8">
-        <v>2</v>
-      </c>
-      <c r="F10" s="8">
-        <v>3</v>
-      </c>
-      <c r="G10" s="8">
-        <v>4</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="10">
+        <v>4</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1116,8 +1117,9 @@
         <v>5</v>
       </c>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1140,8 +1142,9 @@
         <v>5</v>
       </c>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -1164,8 +1167,9 @@
         <v>5</v>
       </c>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -1189,7 +1193,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -1213,7 +1217,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -1617,7 +1621,7 @@
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>9</v>
       </c>
@@ -1641,7 +1645,7 @@
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>10</v>
       </c>
@@ -1665,7 +1669,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>10</v>
       </c>
@@ -1689,7 +1693,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>10</v>
       </c>
@@ -1713,7 +1717,7 @@
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>11</v>
       </c>
@@ -1737,7 +1741,7 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>11</v>
       </c>
@@ -1761,7 +1765,7 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>11</v>
       </c>
@@ -1785,7 +1789,7 @@
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>12</v>
       </c>
@@ -1809,7 +1813,7 @@
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>12</v>
       </c>
@@ -1833,7 +1837,7 @@
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>12</v>
       </c>
@@ -1857,7 +1861,7 @@
       </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>13</v>
       </c>
@@ -1881,7 +1885,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>13</v>
       </c>
@@ -1905,7 +1909,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>13</v>
       </c>
@@ -1928,8 +1932,9 @@
         <v>5</v>
       </c>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>14</v>
       </c>
@@ -1952,8 +1957,9 @@
         <v>5</v>
       </c>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>14</v>
       </c>
@@ -1976,8 +1982,9 @@
         <v>5</v>
       </c>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>15</v>
       </c>
@@ -2001,7 +2008,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>15</v>
       </c>
@@ -2025,7 +2032,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>15</v>
       </c>
@@ -2049,7 +2056,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>16</v>
       </c>
@@ -2073,7 +2080,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>16</v>
       </c>
@@ -2097,7 +2104,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>17</v>
       </c>
@@ -2120,8 +2127,9 @@
         <v>5</v>
       </c>
       <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>17</v>
       </c>
@@ -2144,8 +2152,9 @@
         <v>5</v>
       </c>
       <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>17</v>
       </c>
@@ -2168,8 +2177,9 @@
         <v>5</v>
       </c>
       <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>18</v>
       </c>
@@ -2191,7 +2201,7 @@
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>18</v>
       </c>
@@ -2215,7 +2225,7 @@
       </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>18</v>
       </c>
@@ -2238,8 +2248,9 @@
         <v>5</v>
       </c>
       <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>19</v>
       </c>
@@ -2262,8 +2273,9 @@
         <v>4</v>
       </c>
       <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>19</v>
       </c>
@@ -2286,8 +2298,9 @@
         <v>4</v>
       </c>
       <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>19</v>
       </c>
@@ -2311,7 +2324,7 @@
       </c>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>20</v>
       </c>
@@ -2335,7 +2348,7 @@
       </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>20</v>
       </c>
@@ -2359,7 +2372,7 @@
       </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>20</v>
       </c>
@@ -2383,7 +2396,7 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>21</v>
       </c>
@@ -2407,7 +2420,7 @@
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>21</v>
       </c>
@@ -2431,7 +2444,7 @@
       </c>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>22</v>
       </c>
@@ -2455,7 +2468,7 @@
       </c>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>22</v>
       </c>
@@ -2479,7 +2492,7 @@
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>23</v>
       </c>
@@ -2503,7 +2516,7 @@
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>23</v>
       </c>
@@ -2527,7 +2540,7 @@
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>23</v>
       </c>
@@ -2551,7 +2564,7 @@
       </c>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>24</v>
       </c>
@@ -2572,8 +2585,9 @@
         <v>0</v>
       </c>
       <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>24</v>
       </c>
@@ -2594,8 +2608,9 @@
         <v>0</v>
       </c>
       <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>25</v>
       </c>
@@ -2616,8 +2631,9 @@
         <v>5</v>
       </c>
       <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>25</v>
       </c>
@@ -2641,7 +2657,7 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>26</v>
       </c>
@@ -2665,7 +2681,7 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>26</v>
       </c>
@@ -2689,7 +2705,7 @@
       </c>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>26</v>
       </c>
@@ -2712,8 +2728,9 @@
         <v>5</v>
       </c>
       <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>27</v>
       </c>
@@ -2736,8 +2753,9 @@
         <v>5</v>
       </c>
       <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>27</v>
       </c>
@@ -2760,8 +2778,9 @@
         <v>5</v>
       </c>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>27</v>
       </c>
@@ -2784,8 +2803,9 @@
         <v>5</v>
       </c>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>28</v>
       </c>
@@ -2808,8 +2828,9 @@
         <v>4</v>
       </c>
       <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>28</v>
       </c>
@@ -2833,7 +2854,7 @@
       </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>29</v>
       </c>
@@ -2855,7 +2876,7 @@
       </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>29</v>
       </c>
@@ -2879,7 +2900,7 @@
       </c>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>29</v>
       </c>
@@ -2901,7 +2922,7 @@
       </c>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>30</v>
       </c>
@@ -2925,7 +2946,7 @@
       </c>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>30</v>
       </c>
@@ -2949,7 +2970,7 @@
       </c>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>30</v>
       </c>
@@ -2973,7 +2994,7 @@
       </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>31</v>
       </c>
@@ -2995,7 +3016,7 @@
       </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>31</v>
       </c>
@@ -3017,7 +3038,7 @@
       </c>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>31</v>
       </c>
@@ -3039,7 +3060,7 @@
       </c>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>32</v>
       </c>
@@ -3063,7 +3084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>32</v>
       </c>
@@ -3089,7 +3110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>32</v>
       </c>
@@ -3115,7 +3136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>33</v>
       </c>
@@ -3324,45 +3345,75 @@
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="3"/>
+      <c r="A104" s="3">
+        <v>37</v>
+      </c>
       <c r="B104" s="4">
-        <v>2002104309</v>
+        <v>2011502114</v>
       </c>
       <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
+      <c r="D104" s="1">
+        <v>4</v>
+      </c>
+      <c r="E104" s="1">
+        <v>3</v>
+      </c>
+      <c r="F104" s="1">
+        <v>2</v>
+      </c>
+      <c r="G104" s="1">
+        <v>5</v>
+      </c>
       <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
+      <c r="A105" s="3">
+        <v>37</v>
+      </c>
       <c r="B105" s="4">
-        <v>2010502051</v>
+        <v>2013502180</v>
       </c>
       <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
+      <c r="D105" s="1">
+        <v>4</v>
+      </c>
+      <c r="E105" s="1">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1">
+        <v>2</v>
+      </c>
+      <c r="G105" s="1">
+        <v>5</v>
+      </c>
       <c r="H105" s="1"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="3"/>
+      <c r="A106" s="3">
+        <v>37</v>
+      </c>
       <c r="B106" s="4">
-        <v>2010502153</v>
+        <v>2013502207</v>
       </c>
       <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
+      <c r="D106" s="1">
+        <v>4</v>
+      </c>
+      <c r="E106" s="1">
+        <v>3</v>
+      </c>
+      <c r="F106" s="1">
+        <v>2</v>
+      </c>
+      <c r="G106" s="1">
+        <v>5</v>
+      </c>
       <c r="H106" s="1"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4">
-        <v>2011502114</v>
+        <v>2002104309</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -3374,7 +3425,7 @@
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4">
-        <v>2012502045</v>
+        <v>2010502051</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -3386,7 +3437,7 @@
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4">
-        <v>2012502132</v>
+        <v>2010502153</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -3398,7 +3449,7 @@
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4">
-        <v>2012502177</v>
+        <v>2012502045</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -3410,11 +3461,9 @@
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4">
-        <v>2013502012</v>
-      </c>
-      <c r="C111" s="1">
-        <v>4.5</v>
-      </c>
+        <v>2012502132</v>
+      </c>
+      <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -3424,11 +3473,9 @@
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4">
-        <v>2013502075</v>
-      </c>
-      <c r="C112" s="1">
-        <v>4.75</v>
-      </c>
+        <v>2012502177</v>
+      </c>
+      <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -3438,9 +3485,11 @@
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4">
-        <v>2013502180</v>
-      </c>
-      <c r="C113" s="1"/>
+        <v>2013502012</v>
+      </c>
+      <c r="C113" s="1">
+        <v>4.5</v>
+      </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -3450,9 +3499,11 @@
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4">
-        <v>2013502207</v>
-      </c>
-      <c r="C114" s="1"/>
+        <v>2013502075</v>
+      </c>
+      <c r="C114" s="1">
+        <v>4.75</v>
+      </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>

</xml_diff>

<commit_message>
Quiz 2 announced. Object before Nov 9.
</commit_message>
<xml_diff>
--- a/331GRADES.xlsx
+++ b/331GRADES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Furkan\Desktop\331\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12666D17-5366-4C75-842C-34C7201C628A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD62038E-742C-4A1B-A193-2674982F14AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1005" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="grades" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grades!$A$11:$I$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grades!$A$5:$I$114</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Student ID</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>Each question is graded out of 5. The weights of questions are not determined yet.</t>
   </si>
   <si>
     <t>In Q1, each defined data mining problem is 1 point. The rest is 2 points.</t>
@@ -70,12 +67,30 @@
   <si>
     <t>HW#1</t>
   </si>
+  <si>
+    <t>HW#1 Notes</t>
+  </si>
+  <si>
+    <t>Quiz#2 Notes</t>
+  </si>
+  <si>
+    <t>If your answer was Yes, you get 0 or 1 point based on whether you showed that you more or less understand what is confidence, support, or lift concepts.</t>
+  </si>
+  <si>
+    <t>If your answer was No, and you get less than 5 points, it indicates that there are some errors or insufficiencies in your explanation. Minor calculation mistakes are ignored.</t>
+  </si>
+  <si>
+    <t>Each quiz and homework question is graded out of 5. The weights of homework questions are not determined yet.</t>
+  </si>
+  <si>
+    <t>Notes are below the list. See them before objection.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +254,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -664,7 +687,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -678,9 +700,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1036,16 +1057,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="11.140625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1" collapsed="1"/>
@@ -1054,177 +1076,268 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
+      <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>3</v>
+      </c>
+      <c r="H5" s="10">
+        <v>4</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4">
+        <v>2002104309</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2009502060</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="3">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2010502021</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4">
+        <v>2010502051</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="E10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4">
+        <v>2010502153</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="11">
-        <v>2</v>
-      </c>
-      <c r="G11" s="11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="11">
-        <v>4</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>2</v>
-      </c>
+      <c r="A11" s="3">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2011502114</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4">
-        <v>2015502045</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4.75</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12" s="2">
-        <v>4</v>
-      </c>
-      <c r="H12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="5"/>
+        <v>2011502144</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4">
-        <v>2015502105</v>
+        <v>2011502171</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
       <c r="E13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4">
-        <v>2015502126</v>
+        <v>2011502234</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="1">
         <v>5</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4">
-        <v>2013502138</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
+        <v>2012502042</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H15" s="1">
         <v>5</v>
@@ -1232,49 +1345,35 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>2</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="4">
-        <v>2014502165</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4.75</v>
-      </c>
+        <v>2012502045</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>5</v>
-      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17" s="4">
-        <v>2015502216</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
+        <v>2012502078</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1">
         <v>5</v>
@@ -1283,167 +1382,139 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4">
-        <v>2016502219</v>
-      </c>
-      <c r="C18" s="1">
-        <v>4.75</v>
-      </c>
+        <v>2012502105</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>4</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="4">
-        <v>2014502024</v>
-      </c>
-      <c r="C19" s="1">
-        <v>5</v>
-      </c>
+        <v>2012502132</v>
+      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1">
-        <v>2</v>
-      </c>
-      <c r="F19" s="1">
-        <v>3</v>
-      </c>
-      <c r="G19" s="1">
-        <v>3</v>
-      </c>
-      <c r="H19" s="1">
-        <v>5</v>
-      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B20" s="4">
-        <v>2014502156</v>
-      </c>
-      <c r="C20" s="1">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>2012502168</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
       <c r="E20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1">
         <v>3</v>
       </c>
       <c r="G20" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>5</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="4">
-        <v>2012502078</v>
+        <v>2012502177</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>5</v>
-      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="4">
-        <v>2014502087</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>2013502012</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.5</v>
+      </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>5</v>
-      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4">
-        <v>2017502252</v>
+        <v>2013502018</v>
       </c>
       <c r="C23" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
       <c r="E23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4">
-        <v>2013502165</v>
+        <v>2013502030</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
       <c r="E24" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
         <v>5</v>
@@ -1452,46 +1523,50 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4">
-        <v>2013502171</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+        <v>2013502042</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
       <c r="E25" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B26" s="4">
-        <v>2015502159</v>
+        <v>2013502069</v>
       </c>
       <c r="C26" s="1">
         <v>4.75</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26" s="1">
         <v>5</v>
@@ -1499,28 +1574,20 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>7</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="4">
-        <v>2013502084</v>
+        <v>2013502075</v>
       </c>
       <c r="C27" s="1">
-        <v>5</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1">
-        <v>2</v>
-      </c>
-      <c r="F27" s="1">
-        <v>4</v>
-      </c>
-      <c r="G27" s="1">
-        <v>4</v>
-      </c>
-      <c r="H27" s="1">
-        <v>5</v>
-      </c>
+        <v>4.75</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1528,12 +1595,14 @@
         <v>7</v>
       </c>
       <c r="B28" s="4">
-        <v>2015502165</v>
+        <v>2013502084</v>
       </c>
       <c r="C28" s="1">
         <v>5</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
       <c r="E28" s="1">
         <v>2</v>
       </c>
@@ -1550,26 +1619,28 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B29" s="4">
-        <v>2017502201</v>
+        <v>2013502132</v>
       </c>
       <c r="C29" s="1">
         <v>5</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
       <c r="E29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G29" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -1578,10 +1649,10 @@
         <v>8</v>
       </c>
       <c r="B30" s="4">
-        <v>2013502069</v>
+        <v>2013502135</v>
       </c>
       <c r="C30" s="1">
-        <v>4.75</v>
+        <v>4.25</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1">
@@ -1600,17 +1671,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B31" s="4">
-        <v>2013502135</v>
+        <v>2013502138</v>
       </c>
       <c r="C31" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D31" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
       <c r="E31" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1">
         <v>2</v>
@@ -1625,23 +1698,25 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4">
-        <v>2014502132</v>
+        <v>2013502150</v>
       </c>
       <c r="C32" s="1">
-        <v>5</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>4.75</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5</v>
+      </c>
       <c r="E32" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F32" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H32" s="1">
         <v>5</v>
@@ -1650,96 +1725,100 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B33" s="4">
-        <v>2014502147</v>
+        <v>2013502165</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
       <c r="E33" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F33" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G33" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H33" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B34" s="4">
-        <v>2016502237</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>2013502171</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
       <c r="E34" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G34" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B35" s="4">
-        <v>2015502006</v>
-      </c>
-      <c r="C35" s="1">
-        <v>5</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>2013502180</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
       <c r="E35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G35" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H35" s="1">
         <v>5</v>
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B36" s="4">
-        <v>2015502138</v>
+        <v>2013502183</v>
       </c>
       <c r="C36" s="1">
-        <v>5</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
       <c r="E36" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F36" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G36" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H36" s="1">
         <v>5</v>
@@ -1748,23 +1827,21 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B37" s="4">
-        <v>2016502168</v>
-      </c>
-      <c r="C37" s="1">
-        <v>5</v>
-      </c>
+        <v>2013502207</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G37" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H37" s="1">
         <v>5</v>
@@ -1773,40 +1850,44 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B38" s="4">
-        <v>2014502114</v>
+        <v>2014500024</v>
       </c>
       <c r="C38" s="1">
         <v>5</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
       <c r="E38" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F38" s="1">
         <v>3</v>
       </c>
       <c r="G38" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H38" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B39" s="4">
-        <v>2014502141</v>
+        <v>2014500090</v>
       </c>
       <c r="C39" s="1">
         <v>5</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="1">
+        <v>5</v>
+      </c>
       <c r="E39" s="1">
         <v>4</v>
       </c>
@@ -1814,7 +1895,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H39" s="1">
         <v>5</v>
@@ -1823,20 +1904,22 @@
     </row>
     <row r="40" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B40" s="4">
-        <v>2015502075</v>
+        <v>2014502006</v>
       </c>
       <c r="C40" s="1">
         <v>4.5</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1">
+        <v>5</v>
+      </c>
       <c r="E40" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F40" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G40" s="1">
         <v>3</v>
@@ -1845,6 +1928,7 @@
         <v>5</v>
       </c>
       <c r="I40" s="1"/>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
@@ -1870,41 +1954,45 @@
         <v>5</v>
       </c>
       <c r="I41" s="1"/>
+      <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B42" s="4">
-        <v>2014502030</v>
+        <v>2014502024</v>
       </c>
       <c r="C42" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="D42" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D42" s="1">
+        <v>5</v>
+      </c>
       <c r="E42" s="1">
         <v>2</v>
       </c>
       <c r="F42" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G42" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H42" s="1">
         <v>5</v>
       </c>
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>12</v>
       </c>
       <c r="B43" s="4">
-        <v>2014502048</v>
+        <v>2014502030</v>
       </c>
       <c r="C43" s="1">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1">
@@ -1921,25 +2009,27 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B44" s="4">
-        <v>2014502078</v>
+        <v>2014502045</v>
       </c>
       <c r="C44" s="1">
         <v>5</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
       <c r="E44" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G44" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H44" s="1">
         <v>5</v>
@@ -1948,20 +2038,20 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B45" s="4">
-        <v>2015502015</v>
+        <v>2014502048</v>
       </c>
       <c r="C45" s="1">
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G45" s="1">
         <v>4</v>
@@ -1971,22 +2061,24 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B46" s="4">
-        <v>2015502123</v>
+        <v>2014502051</v>
       </c>
       <c r="C46" s="1">
         <v>5</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="1">
+        <v>5</v>
+      </c>
       <c r="E46" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F46" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G46" s="1">
         <v>4</v>
@@ -1995,24 +2087,21 @@
         <v>5</v>
       </c>
       <c r="I46" s="1"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B47" s="4">
-        <v>2015502150</v>
-      </c>
-      <c r="C47" s="1">
-        <v>4.5</v>
-      </c>
+        <v>2014502063</v>
+      </c>
+      <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F47" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G47" s="1">
         <v>3</v>
@@ -2021,27 +2110,28 @@
         <v>5</v>
       </c>
       <c r="I47" s="1"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B48" s="4">
-        <v>2016502018</v>
+        <v>2014502069</v>
       </c>
       <c r="C48" s="1">
         <v>5</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1">
+        <v>5</v>
+      </c>
       <c r="E48" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G48" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H48" s="1">
         <v>5</v>
@@ -2049,100 +2139,108 @@
       <c r="I48" s="1"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49" s="4">
-        <v>2014502006</v>
+        <v>2014502078</v>
       </c>
       <c r="C49" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D49" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5</v>
+      </c>
       <c r="E49" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F49" s="1">
         <v>2</v>
       </c>
       <c r="G49" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H49" s="1">
         <v>5</v>
       </c>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B50" s="4">
-        <v>2014502162</v>
-      </c>
-      <c r="C50" s="1">
-        <v>5</v>
-      </c>
-      <c r="D50" s="1"/>
+        <v>2014502087</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
       <c r="E50" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F50" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G50" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H50" s="1">
         <v>5</v>
       </c>
       <c r="I50" s="1"/>
+      <c r="J50" s="5"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B51" s="4">
-        <v>2015502120</v>
+        <v>2014502090</v>
       </c>
       <c r="C51" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="D51" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
       <c r="E51" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G51" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H51" s="1">
         <v>5</v>
       </c>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B52" s="4">
-        <v>2015502036</v>
+        <v>2014502093</v>
       </c>
       <c r="C52" s="1">
         <v>4.75</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="1">
+        <v>5</v>
+      </c>
       <c r="E52" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F52" s="1">
         <v>4</v>
       </c>
       <c r="G52" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H52" s="1">
         <v>5</v>
@@ -2151,74 +2249,69 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B53" s="4">
-        <v>2016502225</v>
+        <v>2014502096</v>
       </c>
       <c r="C53" s="1">
         <v>5</v>
       </c>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
       <c r="E53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G53" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H53" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I53" s="1"/>
+      <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>17</v>
-      </c>
+      <c r="A54" s="3"/>
       <c r="B54" s="4">
-        <v>2015502042</v>
+        <v>2014502099</v>
       </c>
       <c r="C54" s="1">
-        <v>5</v>
+        <v>4.25</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="1">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1">
-        <v>4</v>
-      </c>
-      <c r="G54" s="1">
-        <v>4</v>
-      </c>
-      <c r="H54" s="1">
-        <v>5</v>
-      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="5"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B55" s="4">
-        <v>2015502069</v>
+        <v>2014502114</v>
       </c>
       <c r="C55" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D55" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4</v>
+      </c>
       <c r="E55" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F55" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G55" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H55" s="1">
         <v>5</v>
@@ -2228,20 +2321,20 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B56" s="4">
-        <v>2016502051</v>
+        <v>2014502126</v>
       </c>
       <c r="C56" s="1">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G56" s="1">
         <v>4</v>
@@ -2250,25 +2343,28 @@
         <v>5</v>
       </c>
       <c r="I56" s="1"/>
-      <c r="J56" s="5"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B57" s="4">
-        <v>2013502030</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+        <v>2014502132</v>
+      </c>
+      <c r="C57" s="1">
+        <v>5</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
       <c r="E57" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="1">
         <v>5</v>
@@ -2277,148 +2373,151 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B58" s="4">
-        <v>2013502183</v>
+        <v>2014502135</v>
       </c>
       <c r="C58" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B59" s="4">
-        <v>2015502033</v>
+        <v>2014502141</v>
       </c>
       <c r="C59" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D59" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D59" s="1">
+        <v>4</v>
+      </c>
       <c r="E59" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F59" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G59" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H59" s="1">
         <v>5</v>
       </c>
       <c r="I59" s="1"/>
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B60" s="4">
-        <v>2014500024</v>
-      </c>
-      <c r="C60" s="1">
-        <v>5</v>
-      </c>
+        <v>2014502147</v>
+      </c>
+      <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1">
         <v>1</v>
       </c>
       <c r="F60" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I60" s="1"/>
-      <c r="J60" s="5"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B61" s="4">
-        <v>2014502096</v>
+        <v>2014502150</v>
       </c>
       <c r="C61" s="1">
         <v>5</v>
       </c>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1">
+        <v>5</v>
+      </c>
       <c r="E61" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F61" s="1">
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H61" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I61" s="1"/>
-      <c r="J61" s="5"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B62" s="4">
-        <v>2015502228</v>
-      </c>
-      <c r="C62" s="1">
-        <v>5</v>
-      </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1">
-        <v>1</v>
-      </c>
-      <c r="F62" s="1">
-        <v>3</v>
-      </c>
-      <c r="G62" s="1">
-        <v>0</v>
-      </c>
-      <c r="H62" s="1">
-        <v>4</v>
-      </c>
-      <c r="I62" s="1"/>
+        <v>2014502156</v>
+      </c>
+      <c r="C62" s="2">
+        <v>3</v>
+      </c>
+      <c r="D62" s="2">
+        <v>5</v>
+      </c>
+      <c r="E62" s="2">
+        <v>2</v>
+      </c>
+      <c r="F62" s="2">
+        <v>3</v>
+      </c>
+      <c r="G62" s="2">
+        <v>3</v>
+      </c>
+      <c r="H62" s="2">
+        <v>5</v>
+      </c>
+      <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B63" s="4">
-        <v>2015502063</v>
+        <v>2014502162</v>
       </c>
       <c r="C63" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D63" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D63" s="1">
+        <v>5</v>
+      </c>
       <c r="E63" s="1">
         <v>1</v>
       </c>
       <c r="F63" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G63" s="1">
         <v>3</v>
@@ -2430,23 +2529,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B64" s="4">
-        <v>2015502156</v>
+        <v>2014502165</v>
       </c>
       <c r="C64" s="1">
-        <v>5</v>
-      </c>
-      <c r="D64" s="1"/>
+        <v>4.75</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
       <c r="E64" s="1">
         <v>1</v>
       </c>
       <c r="F64" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G64" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H64" s="1">
         <v>5</v>
@@ -2455,145 +2556,142 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B65" s="4">
-        <v>2015502171</v>
-      </c>
-      <c r="C65" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D65" s="1"/>
+        <v>2014502168</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1">
+        <v>5</v>
+      </c>
       <c r="E65" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F65" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G65" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H65" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:10" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
-        <v>21</v>
-      </c>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
       <c r="B66" s="4">
-        <v>2014500090</v>
+        <v>2014502177</v>
       </c>
       <c r="C66" s="1">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D66" s="1"/>
-      <c r="E66" s="1">
-        <v>4</v>
-      </c>
-      <c r="F66" s="1">
-        <v>3</v>
-      </c>
-      <c r="G66" s="1">
-        <v>2</v>
-      </c>
-      <c r="H66" s="1">
-        <v>5</v>
-      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B67" s="4">
-        <v>2015502108</v>
-      </c>
-      <c r="C67" s="1">
-        <v>4.25</v>
-      </c>
+        <v>2014502183</v>
+      </c>
+      <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F67" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G67" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H67" s="1">
         <v>5</v>
       </c>
       <c r="I67" s="1"/>
+      <c r="J67" s="5"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B68" s="4">
-        <v>2014502045</v>
-      </c>
-      <c r="C68" s="2">
-        <v>5</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2">
-        <v>5</v>
-      </c>
-      <c r="F68" s="2">
-        <v>3</v>
-      </c>
-      <c r="G68" s="2">
-        <v>5</v>
-      </c>
-      <c r="H68" s="2">
-        <v>5</v>
-      </c>
-      <c r="I68" s="2"/>
+        <v>2015502006</v>
+      </c>
+      <c r="C68" s="1">
+        <v>5</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1">
+        <v>3</v>
+      </c>
+      <c r="F68" s="1">
+        <v>4</v>
+      </c>
+      <c r="G68" s="1">
+        <v>4</v>
+      </c>
+      <c r="H68" s="1">
+        <v>5</v>
+      </c>
+      <c r="I68" s="1"/>
+      <c r="J68" s="5"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B69" s="4">
-        <v>2014502150</v>
+        <v>2015502009</v>
       </c>
       <c r="C69" s="1">
-        <v>5</v>
-      </c>
-      <c r="D69" s="1"/>
+        <v>4.25</v>
+      </c>
+      <c r="D69" s="1">
+        <v>5</v>
+      </c>
       <c r="E69" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F69" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G69" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H69" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I69" s="1"/>
+      <c r="J69" s="5"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B70" s="4">
-        <v>2014502069</v>
+        <v>2015502015</v>
       </c>
       <c r="C70" s="1">
-        <v>5</v>
-      </c>
-      <c r="D70" s="1"/>
+        <v>4.75</v>
+      </c>
+      <c r="D70" s="1">
+        <v>2</v>
+      </c>
       <c r="E70" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F70" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G70" s="1">
         <v>4</v>
@@ -2604,41 +2702,31 @@
       <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
-        <v>23</v>
-      </c>
+      <c r="A71" s="3"/>
       <c r="B71" s="4">
-        <v>2014502090</v>
-      </c>
-      <c r="C71" s="1">
-        <v>5</v>
-      </c>
+        <v>2015502021</v>
+      </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="1">
-        <v>4</v>
-      </c>
-      <c r="F71" s="1">
-        <v>3</v>
-      </c>
-      <c r="G71" s="1">
-        <v>4</v>
-      </c>
-      <c r="H71" s="1">
-        <v>5</v>
-      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B72" s="4">
-        <v>2014502126</v>
+        <v>2015502024</v>
       </c>
       <c r="C72" s="1">
         <v>5</v>
       </c>
-      <c r="D72" s="1"/>
+      <c r="D72" s="1">
+        <v>5</v>
+      </c>
       <c r="E72" s="1">
         <v>4</v>
       </c>
@@ -2655,69 +2743,81 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B73" s="4">
-        <v>2012502168</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+        <v>2015502027</v>
+      </c>
+      <c r="C73" s="1">
+        <v>5</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
       <c r="E73" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F73" s="1">
         <v>3</v>
       </c>
       <c r="G73" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H73" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I73" s="1"/>
       <c r="J73" s="5"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B74" s="4">
-        <v>2014502168</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+        <v>2015502033</v>
+      </c>
+      <c r="C74" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D74" s="1">
+        <v>5</v>
+      </c>
       <c r="E74" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F74" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G74" s="1">
         <v>0</v>
       </c>
       <c r="H74" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I74" s="1"/>
       <c r="J74" s="5"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B75" s="4">
-        <v>2016502210</v>
-      </c>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
+        <v>2015502036</v>
+      </c>
+      <c r="C75" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="D75" s="1">
+        <v>5</v>
+      </c>
       <c r="E75" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F75" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G75" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H75" s="1">
         <v>5</v>
@@ -2727,20 +2827,22 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B76" s="4">
-        <v>2017502219</v>
+        <v>2015502039</v>
       </c>
       <c r="C76" s="1">
-        <v>4</v>
-      </c>
-      <c r="D76" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>5</v>
+      </c>
       <c r="E76" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F76" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G76" s="1">
         <v>4</v>
@@ -2749,20 +2851,21 @@
         <v>5</v>
       </c>
       <c r="I76" s="1"/>
+      <c r="J76" s="5"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B77" s="4">
-        <v>2015502039</v>
+        <v>2015502042</v>
       </c>
       <c r="C77" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F77" s="1">
         <v>4</v>
@@ -2774,23 +2877,26 @@
         <v>5</v>
       </c>
       <c r="I77" s="1"/>
+      <c r="J77" s="5"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B78" s="4">
-        <v>2015502090</v>
+        <v>2015502045</v>
       </c>
       <c r="C78" s="1">
-        <v>4</v>
-      </c>
-      <c r="D78" s="1"/>
+        <v>4.75</v>
+      </c>
+      <c r="D78" s="1">
+        <v>5</v>
+      </c>
       <c r="E78" s="1">
         <v>3</v>
       </c>
       <c r="F78" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G78" s="1">
         <v>4</v>
@@ -2802,98 +2908,103 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B79" s="4">
-        <v>2015502147</v>
+        <v>2015502051</v>
       </c>
       <c r="C79" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D79" s="1">
+        <v>5</v>
+      </c>
       <c r="E79" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G79" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H79" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I79" s="1"/>
-      <c r="J79" s="5"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B80" s="4">
-        <v>2015502024</v>
+        <v>2015502060</v>
       </c>
       <c r="C80" s="1">
         <v>5</v>
       </c>
-      <c r="D80" s="1"/>
+      <c r="D80" s="1">
+        <v>5</v>
+      </c>
       <c r="E80" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F80" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G80" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H80" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I80" s="1"/>
-      <c r="J80" s="5"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B81" s="4">
-        <v>2015502027</v>
+        <v>2015502063</v>
       </c>
       <c r="C81" s="1">
-        <v>5</v>
-      </c>
-      <c r="D81" s="1"/>
+        <v>4.25</v>
+      </c>
+      <c r="D81" s="1">
+        <v>4</v>
+      </c>
       <c r="E81" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F81" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G81" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H81" s="1">
         <v>5</v>
       </c>
       <c r="I81" s="1"/>
-      <c r="J81" s="5"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B82" s="4">
-        <v>2015502207</v>
+        <v>2015502069</v>
       </c>
       <c r="C82" s="1">
         <v>4.5</v>
       </c>
-      <c r="D82" s="1"/>
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
       <c r="E82" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F82" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G82" s="1">
         <v>4</v>
@@ -2902,265 +3013,291 @@
         <v>5</v>
       </c>
       <c r="I82" s="1"/>
-      <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B83" s="4">
-        <v>2015502051</v>
+        <v>2015502075</v>
       </c>
       <c r="C83" s="1">
-        <v>5</v>
-      </c>
-      <c r="D83" s="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="D83" s="1">
+        <v>5</v>
+      </c>
       <c r="E83" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F83" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G83" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H83" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I83" s="1"/>
-      <c r="J83" s="5"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B84" s="4">
-        <v>2015502060</v>
+        <v>2015502090</v>
       </c>
       <c r="C84" s="1">
-        <v>5</v>
-      </c>
-      <c r="D84" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
       <c r="E84" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F84" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G84" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
+        <v>1</v>
+      </c>
+      <c r="B85" s="4">
+        <v>2015502105</v>
+      </c>
+      <c r="C85" s="1">
+        <v>4</v>
+      </c>
+      <c r="D85" s="1">
+        <v>5</v>
+      </c>
+      <c r="E85" s="1">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1">
+        <v>3</v>
+      </c>
+      <c r="G85" s="1">
+        <v>4</v>
+      </c>
+      <c r="H85" s="1">
+        <v>5</v>
+      </c>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>21</v>
+      </c>
+      <c r="B86" s="4">
+        <v>2015502108</v>
+      </c>
+      <c r="C86" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+      <c r="E86" s="1">
+        <v>4</v>
+      </c>
+      <c r="F86" s="1">
+        <v>3</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2</v>
+      </c>
+      <c r="H86" s="1">
+        <v>5</v>
+      </c>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>15</v>
+      </c>
+      <c r="B87" s="4">
+        <v>2015502120</v>
+      </c>
+      <c r="C87" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="D87" s="1">
+        <v>5</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1">
+        <v>2</v>
+      </c>
+      <c r="G87" s="1">
+        <v>3</v>
+      </c>
+      <c r="H87" s="1">
+        <v>5</v>
+      </c>
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>13</v>
+      </c>
+      <c r="B88" s="4">
+        <v>2015502123</v>
+      </c>
+      <c r="C88" s="1">
+        <v>5</v>
+      </c>
+      <c r="D88" s="1">
+        <v>5</v>
+      </c>
+      <c r="E88" s="1">
+        <v>3</v>
+      </c>
+      <c r="F88" s="1">
+        <v>2</v>
+      </c>
+      <c r="G88" s="1">
+        <v>4</v>
+      </c>
+      <c r="H88" s="1">
+        <v>5</v>
+      </c>
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>1</v>
+      </c>
+      <c r="B89" s="4">
+        <v>2015502126</v>
+      </c>
+      <c r="C89" s="1">
+        <v>5</v>
+      </c>
+      <c r="D89" s="1">
+        <v>5</v>
+      </c>
+      <c r="E89" s="1">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3</v>
+      </c>
+      <c r="G89" s="1">
+        <v>4</v>
+      </c>
+      <c r="H89" s="1">
+        <v>5</v>
+      </c>
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>10</v>
+      </c>
+      <c r="B90" s="4">
+        <v>2015502138</v>
+      </c>
+      <c r="C90" s="1">
+        <v>5</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1</v>
+      </c>
+      <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>4</v>
+      </c>
+      <c r="G90" s="1">
+        <v>4</v>
+      </c>
+      <c r="H90" s="1">
+        <v>5</v>
+      </c>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
         <v>29</v>
       </c>
-      <c r="B85" s="4">
-        <v>2009502060</v>
-      </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1">
-        <v>2</v>
-      </c>
-      <c r="F85" s="1">
-        <v>0</v>
-      </c>
-      <c r="G85" s="1">
-        <v>5</v>
-      </c>
-      <c r="H85" s="1">
-        <v>3</v>
-      </c>
-      <c r="I85" s="1"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
-        <v>29</v>
-      </c>
-      <c r="B86" s="4">
-        <v>2011502171</v>
-      </c>
-      <c r="C86" s="1">
-        <v>3</v>
-      </c>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1">
-        <v>2</v>
-      </c>
-      <c r="F86" s="1">
-        <v>0</v>
-      </c>
-      <c r="G86" s="1">
-        <v>5</v>
-      </c>
-      <c r="H86" s="1">
-        <v>3</v>
-      </c>
-      <c r="I86" s="1"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
-        <v>29</v>
-      </c>
-      <c r="B87" s="4">
+      <c r="B91" s="4">
         <v>2015502141</v>
-      </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1">
-        <v>2</v>
-      </c>
-      <c r="F87" s="1">
-        <v>0</v>
-      </c>
-      <c r="G87" s="1">
-        <v>5</v>
-      </c>
-      <c r="H87" s="1">
-        <v>3</v>
-      </c>
-      <c r="I87" s="1"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="3">
-        <v>30</v>
-      </c>
-      <c r="B88" s="4">
-        <v>2013502150</v>
-      </c>
-      <c r="C88" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1">
-        <v>5</v>
-      </c>
-      <c r="F88" s="1">
-        <v>4</v>
-      </c>
-      <c r="G88" s="1">
-        <v>4</v>
-      </c>
-      <c r="H88" s="1">
-        <v>5</v>
-      </c>
-      <c r="I88" s="1"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3">
-        <v>30</v>
-      </c>
-      <c r="B89" s="4">
-        <v>2014502051</v>
-      </c>
-      <c r="C89" s="1">
-        <v>5</v>
-      </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1">
-        <v>5</v>
-      </c>
-      <c r="F89" s="1">
-        <v>4</v>
-      </c>
-      <c r="G89" s="1">
-        <v>4</v>
-      </c>
-      <c r="H89" s="1">
-        <v>5</v>
-      </c>
-      <c r="I89" s="1"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
-        <v>30</v>
-      </c>
-      <c r="B90" s="4">
-        <v>2014502093</v>
-      </c>
-      <c r="C90" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1">
-        <v>5</v>
-      </c>
-      <c r="F90" s="1">
-        <v>4</v>
-      </c>
-      <c r="G90" s="1">
-        <v>4</v>
-      </c>
-      <c r="H90" s="1">
-        <v>5</v>
-      </c>
-      <c r="I90" s="1"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
-        <v>31</v>
-      </c>
-      <c r="B91" s="4">
-        <v>2012502042</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H91" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B92" s="4">
-        <v>2014502063</v>
-      </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+        <v>2015502147</v>
+      </c>
+      <c r="C92" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="D92" s="1">
+        <v>5</v>
+      </c>
       <c r="E92" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F92" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G92" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H92" s="1">
         <v>5</v>
       </c>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B93" s="4">
-        <v>2014502183</v>
-      </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
+        <v>2015502150</v>
+      </c>
+      <c r="C93" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D93" s="1">
+        <v>5</v>
+      </c>
       <c r="E93" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F93" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G93" s="1">
         <v>3</v>
@@ -3170,273 +3307,281 @@
       </c>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B94" s="4">
-        <v>2012502105</v>
-      </c>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
+        <v>2015502156</v>
+      </c>
+      <c r="C94" s="1">
+        <v>5</v>
+      </c>
+      <c r="D94" s="1">
+        <v>5</v>
+      </c>
       <c r="E94" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G94" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B95" s="4">
-        <v>2013502042</v>
+        <v>2015502159</v>
       </c>
       <c r="C95" s="1">
-        <v>5</v>
-      </c>
-      <c r="D95" s="1"/>
+        <v>4.75</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1</v>
+      </c>
       <c r="E95" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F95" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G95" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H95" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B96" s="4">
-        <v>2014502135</v>
+        <v>2015502165</v>
       </c>
       <c r="C96" s="1">
         <v>5</v>
       </c>
-      <c r="D96" s="1"/>
+      <c r="D96" s="1">
+        <v>5</v>
+      </c>
       <c r="E96" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F96" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G96" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H96" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I96" s="1"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B97" s="4">
-        <v>2013502018</v>
+        <v>2015502171</v>
       </c>
       <c r="C97" s="1">
-        <v>5</v>
+        <v>4.25</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1">
         <v>1</v>
       </c>
       <c r="F97" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H97" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B98" s="4">
-        <v>2013502132</v>
+        <v>2015502183</v>
       </c>
       <c r="C98" s="1">
         <v>5</v>
       </c>
-      <c r="D98" s="1"/>
+      <c r="D98" s="1">
+        <v>4</v>
+      </c>
       <c r="E98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H98" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I98" s="1"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B99" s="4">
-        <v>2015502240</v>
+        <v>2015502207</v>
       </c>
       <c r="C99" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D99" s="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
       <c r="E99" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F99" s="1">
         <v>3</v>
       </c>
       <c r="G99" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H99" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I99" s="1"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B100" s="4">
-        <v>2015502009</v>
+        <v>2015502216</v>
       </c>
       <c r="C100" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D100" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D100" s="1">
+        <v>5</v>
+      </c>
       <c r="E100" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F100" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G100" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H100" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B101" s="4">
-        <v>2015502183</v>
+        <v>2015502228</v>
       </c>
       <c r="C101" s="1">
         <v>5</v>
       </c>
-      <c r="D101" s="1"/>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
       <c r="E101" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G101" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H101" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I101" s="1"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B102" s="4">
-        <v>2011502144</v>
+        <v>2015502240</v>
       </c>
       <c r="C102" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D102" s="1"/>
+        <v>4.25</v>
+      </c>
+      <c r="D102" s="1">
+        <v>3</v>
+      </c>
       <c r="E102" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F102" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G102" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H102" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I102" s="1"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="3">
-        <v>35</v>
-      </c>
+      <c r="A103" s="3"/>
       <c r="B103" s="4">
-        <v>2011502234</v>
-      </c>
-      <c r="C103" s="1">
-        <v>4.75</v>
-      </c>
+        <v>2016502000</v>
+      </c>
+      <c r="C103" s="1"/>
       <c r="D103" s="1"/>
-      <c r="E103" s="1">
-        <v>4</v>
-      </c>
-      <c r="F103" s="1">
-        <v>0</v>
-      </c>
-      <c r="G103" s="1">
-        <v>3</v>
-      </c>
-      <c r="H103" s="1">
-        <v>5</v>
-      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B104" s="4">
-        <v>2010502021</v>
+        <v>2016502018</v>
       </c>
       <c r="C104" s="1">
-        <v>1</v>
-      </c>
-      <c r="D104" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D104" s="1">
+        <v>3</v>
+      </c>
       <c r="E104" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G104" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H104" s="1">
         <v>5</v>
@@ -3445,18 +3590,20 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B105" s="4">
-        <v>2011502114</v>
-      </c>
-      <c r="C105" s="1"/>
+        <v>2016502051</v>
+      </c>
+      <c r="C105" s="1">
+        <v>4.75</v>
+      </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F105" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G105" s="1">
         <v>4</v>
@@ -3468,21 +3615,25 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B106" s="4">
-        <v>2013502180</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
+        <v>2016502168</v>
+      </c>
+      <c r="C106" s="1">
+        <v>5</v>
+      </c>
+      <c r="D106" s="1">
+        <v>5</v>
+      </c>
       <c r="E106" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F106" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G106" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H106" s="1">
         <v>5</v>
@@ -3491,21 +3642,21 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B107" s="4">
-        <v>2013502207</v>
+        <v>2016502210</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F107" s="1">
         <v>3</v>
       </c>
       <c r="G107" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H107" s="1">
         <v>5</v>
@@ -3515,10 +3666,12 @@
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4">
-        <v>2002104309</v>
+        <v>2016502213</v>
       </c>
       <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -3526,179 +3679,219 @@
       <c r="I108" s="1"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="3"/>
+      <c r="A109" s="3">
+        <v>3</v>
+      </c>
       <c r="B109" s="4">
-        <v>2010502051</v>
-      </c>
-      <c r="C109" s="1"/>
+        <v>2016502219</v>
+      </c>
+      <c r="C109" s="1">
+        <v>4.75</v>
+      </c>
       <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
+      <c r="E109" s="1">
+        <v>2</v>
+      </c>
+      <c r="F109" s="1">
+        <v>2</v>
+      </c>
+      <c r="G109" s="1">
+        <v>5</v>
+      </c>
+      <c r="H109" s="1">
+        <v>5</v>
+      </c>
       <c r="I109" s="1"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="3"/>
+      <c r="A110" s="3">
+        <v>16</v>
+      </c>
       <c r="B110" s="4">
-        <v>2010502153</v>
-      </c>
-      <c r="C110" s="1"/>
+        <v>2016502225</v>
+      </c>
+      <c r="C110" s="1">
+        <v>5</v>
+      </c>
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
+      <c r="E110" s="1">
+        <v>2</v>
+      </c>
+      <c r="F110" s="1">
+        <v>4</v>
+      </c>
+      <c r="G110" s="1">
+        <v>3</v>
+      </c>
+      <c r="H110" s="1">
+        <v>5</v>
+      </c>
       <c r="I110" s="1"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="3"/>
+      <c r="A111" s="3">
+        <v>9</v>
+      </c>
       <c r="B111" s="4">
-        <v>2012502045</v>
-      </c>
-      <c r="C111" s="1"/>
+        <v>2016502237</v>
+      </c>
+      <c r="C111" s="1">
+        <v>2</v>
+      </c>
       <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1">
+        <v>4</v>
+      </c>
+      <c r="G111" s="1">
+        <v>1</v>
+      </c>
+      <c r="H111" s="1">
+        <v>1</v>
+      </c>
       <c r="I111" s="1"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="3"/>
+      <c r="A112" s="3">
+        <v>7</v>
+      </c>
       <c r="B112" s="4">
-        <v>2012502132</v>
-      </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
+        <v>2017502201</v>
+      </c>
+      <c r="C112" s="1">
+        <v>5</v>
+      </c>
+      <c r="D112" s="1">
+        <v>5</v>
+      </c>
+      <c r="E112" s="1">
+        <v>2</v>
+      </c>
+      <c r="F112" s="1">
+        <v>4</v>
+      </c>
+      <c r="G112" s="1">
+        <v>4</v>
+      </c>
+      <c r="H112" s="1">
+        <v>5</v>
+      </c>
       <c r="I112" s="1"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
+      <c r="A113" s="3">
+        <v>25</v>
+      </c>
       <c r="B113" s="4">
-        <v>2012502177</v>
-      </c>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
+        <v>2017502219</v>
+      </c>
+      <c r="C113" s="1">
+        <v>4</v>
+      </c>
+      <c r="D113" s="1">
+        <v>3</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+      <c r="F113" s="1">
+        <v>3</v>
+      </c>
+      <c r="G113" s="1">
+        <v>4</v>
+      </c>
+      <c r="H113" s="1">
+        <v>5</v>
+      </c>
       <c r="I113" s="1"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="3"/>
+      <c r="A114" s="3">
+        <v>5</v>
+      </c>
       <c r="B114" s="4">
-        <v>2013502012</v>
+        <v>2017502252</v>
       </c>
       <c r="C114" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
+        <v>4.25</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1</v>
+      </c>
+      <c r="E114" s="1">
+        <v>2</v>
+      </c>
+      <c r="F114" s="1">
+        <v>0</v>
+      </c>
+      <c r="G114" s="1">
+        <v>1</v>
+      </c>
+      <c r="H114" s="1">
+        <v>5</v>
+      </c>
       <c r="I114" s="1"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="3"/>
-      <c r="B115" s="4">
-        <v>2013502075</v>
-      </c>
-      <c r="C115" s="1">
-        <v>4.75</v>
-      </c>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="3"/>
-      <c r="B116" s="4">
-        <v>2014502099</v>
-      </c>
-      <c r="C116" s="1">
-        <v>4.25</v>
-      </c>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-      <c r="I116" s="1"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
-      <c r="B117" s="4">
-        <v>2014502177</v>
-      </c>
-      <c r="C117" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-      <c r="G117" s="1"/>
-      <c r="H117" s="1"/>
-      <c r="I117" s="1"/>
-    </row>
+    <row r="115" spans="1:9" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="4">
-        <v>2015502021</v>
-      </c>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="1"/>
+      <c r="A118" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
-      <c r="B119" s="4">
-        <v>2016502000</v>
-      </c>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="1"/>
+      <c r="A119" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="3"/>
-      <c r="B120" s="4">
-        <v>2016502213</v>
-      </c>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="1"/>
-    </row>
-    <row r="121" spans="1:9" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="A120" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A11:I120" xr:uid="{3B85C355-8385-4A74-A08B-58A7111B11CA}">
-    <sortState ref="A12:I120">
-      <sortCondition ref="A11:A120"/>
+  <autoFilter ref="A5:I114" xr:uid="{3B85C355-8385-4A74-A08B-58A7111B11CA}">
+    <sortState ref="A6:I114">
+      <sortCondition ref="B5:B114"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E4:H4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
HW#2 and Quiz#3 grades are announced.
</commit_message>
<xml_diff>
--- a/331GRADES.xlsx
+++ b/331GRADES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Furkan\Desktop\331\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0011F75-BB88-4C43-86E6-531F703C2087}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E918A6DA-FD28-4543-B8FD-2FB28EAD3F6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1005" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,12 +836,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -862,6 +856,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:N137"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,17 +1259,17 @@
     <row r="5" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="13" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1281,13 +1281,13 @@
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -1296,19 +1296,19 @@
       <c r="H7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="2">
         <v>3</v>
       </c>
@@ -1338,9 +1338,15 @@
       <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="J8" s="4">
+        <v>5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>5</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4.5</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="5"/>
     </row>
@@ -1370,9 +1376,15 @@
       <c r="I9" s="1">
         <v>5</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="J9" s="4">
+        <v>5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4">
+        <v>4.5</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="5"/>
     </row>
@@ -1402,9 +1414,15 @@
       <c r="I10" s="1">
         <v>5</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+      <c r="K10" s="4">
+        <v>5</v>
+      </c>
+      <c r="L10" s="4">
+        <v>4.5</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="5"/>
     </row>

</xml_diff>